<commit_message>
Updated python trading to use jump range
</commit_message>
<xml_diff>
--- a/mission_logs.xlsx
+++ b/mission_logs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -184,10 +184,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -316,6 +316,33 @@
         <v>133533.473684211</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>44141</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>0.704861111111111</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>0.716666666666667</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>1232064</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <f aca="false">G5/F5</f>
+        <v>72474.3529411765</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>